<commit_message>
Regenerate merged AHB files
</commit_message>
<xml_diff>
--- a/data/output/FV2304_FV2210/COMDIS/29001.xlsx
+++ b/data/output/FV2304_FV2210/COMDIS/29001.xlsx
@@ -14,69 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="190">
-  <si>
-    <t>Segmentname_old</t>
-  </si>
-  <si>
-    <t>Segmentgruppe_old</t>
-  </si>
-  <si>
-    <t>Segment_old</t>
-  </si>
-  <si>
-    <t>Datenelement_old</t>
-  </si>
-  <si>
-    <t>Segment ID_old</t>
-  </si>
-  <si>
-    <t>Code_old</t>
-  </si>
-  <si>
-    <t>Qualifier_old</t>
-  </si>
-  <si>
-    <t>Beschreibung_old</t>
-  </si>
-  <si>
-    <t>Bedingungsausdruck_old</t>
-  </si>
-  <si>
-    <t>Bedingung_old</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="190">
+  <si>
+    <t>Segmentname_FV2210</t>
+  </si>
+  <si>
+    <t>Segmentgruppe_FV2210</t>
+  </si>
+  <si>
+    <t>Segment_FV2210</t>
+  </si>
+  <si>
+    <t>Datenelement_FV2210</t>
+  </si>
+  <si>
+    <t>Segment ID_FV2210</t>
+  </si>
+  <si>
+    <t>Code_FV2210</t>
+  </si>
+  <si>
+    <t>Qualifier_FV2210</t>
+  </si>
+  <si>
+    <t>Beschreibung_FV2210</t>
+  </si>
+  <si>
+    <t>Bedingungsausdruck_FV2210</t>
+  </si>
+  <si>
+    <t>Bedingung_FV2210</t>
   </si>
   <si>
     <t>diff</t>
   </si>
   <si>
-    <t>Segmentname_new</t>
-  </si>
-  <si>
-    <t>Segmentgruppe_new</t>
-  </si>
-  <si>
-    <t>Segment_new</t>
-  </si>
-  <si>
-    <t>Datenelement_new</t>
-  </si>
-  <si>
-    <t>Segment ID_new</t>
-  </si>
-  <si>
-    <t>Code_new</t>
-  </si>
-  <si>
-    <t>Qualifier_new</t>
-  </si>
-  <si>
-    <t>Beschreibung_new</t>
-  </si>
-  <si>
-    <t>Bedingungsausdruck_new</t>
-  </si>
-  <si>
-    <t>Bedingung_new</t>
+    <t>Segmentname_FV2304</t>
+  </si>
+  <si>
+    <t>Segmentgruppe_FV2304</t>
+  </si>
+  <si>
+    <t>Segment_FV2304</t>
+  </si>
+  <si>
+    <t>Datenelement_FV2304</t>
+  </si>
+  <si>
+    <t>Segment ID_FV2304</t>
+  </si>
+  <si>
+    <t>Code_FV2304</t>
+  </si>
+  <si>
+    <t>Qualifier_FV2304</t>
+  </si>
+  <si>
+    <t>Beschreibung_FV2304</t>
+  </si>
+  <si>
+    <t>Bedingungsausdruck_FV2304</t>
+  </si>
+  <si>
+    <t>Bedingung_FV2304</t>
   </si>
   <si>
     <t>Nachrichten-Kopfsegment</t>
@@ -675,6 +675,36 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U74" totalsRowShown="0">
+  <autoFilter ref="A1:U74"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Segmentname_FV2210"/>
+    <tableColumn id="2" name="Segmentgruppe_FV2210"/>
+    <tableColumn id="3" name="Segment_FV2210"/>
+    <tableColumn id="4" name="Datenelement_FV2210"/>
+    <tableColumn id="5" name="Segment ID_FV2210"/>
+    <tableColumn id="6" name="Code_FV2210"/>
+    <tableColumn id="7" name="Qualifier_FV2210"/>
+    <tableColumn id="8" name="Beschreibung_FV2210"/>
+    <tableColumn id="9" name="Bedingungsausdruck_FV2210"/>
+    <tableColumn id="10" name="Bedingung_FV2210"/>
+    <tableColumn id="11" name="diff"/>
+    <tableColumn id="12" name="Segmentname_FV2304"/>
+    <tableColumn id="13" name="Segmentgruppe_FV2304"/>
+    <tableColumn id="14" name="Segment_FV2304"/>
+    <tableColumn id="15" name="Datenelement_FV2304"/>
+    <tableColumn id="16" name="Segment ID_FV2304"/>
+    <tableColumn id="17" name="Code_FV2304"/>
+    <tableColumn id="18" name="Qualifier_FV2304"/>
+    <tableColumn id="19" name="Beschreibung_FV2304"/>
+    <tableColumn id="20" name="Bedingungsausdruck_FV2304"/>
+    <tableColumn id="21" name="Bedingung_FV2304"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -964,7 +994,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4393,5 +4426,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: adapt column header formatting to respective input file names (#7)
* Add project descriptions to readme

* Update readme `output.png` path

* Use `<formatversion>` as suffix for table headers

* Add conftest and adjust tests to `<formatversion>` header namings

* Adjust `xlsx` export to new header formatting

* Regenerate merged AHB files
</commit_message>
<xml_diff>
--- a/data/output/FV2304_FV2210/COMDIS/29001.xlsx
+++ b/data/output/FV2304_FV2210/COMDIS/29001.xlsx
@@ -14,69 +14,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="190">
-  <si>
-    <t>Segmentname_old</t>
-  </si>
-  <si>
-    <t>Segmentgruppe_old</t>
-  </si>
-  <si>
-    <t>Segment_old</t>
-  </si>
-  <si>
-    <t>Datenelement_old</t>
-  </si>
-  <si>
-    <t>Segment ID_old</t>
-  </si>
-  <si>
-    <t>Code_old</t>
-  </si>
-  <si>
-    <t>Qualifier_old</t>
-  </si>
-  <si>
-    <t>Beschreibung_old</t>
-  </si>
-  <si>
-    <t>Bedingungsausdruck_old</t>
-  </si>
-  <si>
-    <t>Bedingung_old</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="190">
+  <si>
+    <t>Segmentname_FV2210</t>
+  </si>
+  <si>
+    <t>Segmentgruppe_FV2210</t>
+  </si>
+  <si>
+    <t>Segment_FV2210</t>
+  </si>
+  <si>
+    <t>Datenelement_FV2210</t>
+  </si>
+  <si>
+    <t>Segment ID_FV2210</t>
+  </si>
+  <si>
+    <t>Code_FV2210</t>
+  </si>
+  <si>
+    <t>Qualifier_FV2210</t>
+  </si>
+  <si>
+    <t>Beschreibung_FV2210</t>
+  </si>
+  <si>
+    <t>Bedingungsausdruck_FV2210</t>
+  </si>
+  <si>
+    <t>Bedingung_FV2210</t>
   </si>
   <si>
     <t>diff</t>
   </si>
   <si>
-    <t>Segmentname_new</t>
-  </si>
-  <si>
-    <t>Segmentgruppe_new</t>
-  </si>
-  <si>
-    <t>Segment_new</t>
-  </si>
-  <si>
-    <t>Datenelement_new</t>
-  </si>
-  <si>
-    <t>Segment ID_new</t>
-  </si>
-  <si>
-    <t>Code_new</t>
-  </si>
-  <si>
-    <t>Qualifier_new</t>
-  </si>
-  <si>
-    <t>Beschreibung_new</t>
-  </si>
-  <si>
-    <t>Bedingungsausdruck_new</t>
-  </si>
-  <si>
-    <t>Bedingung_new</t>
+    <t>Segmentname_FV2304</t>
+  </si>
+  <si>
+    <t>Segmentgruppe_FV2304</t>
+  </si>
+  <si>
+    <t>Segment_FV2304</t>
+  </si>
+  <si>
+    <t>Datenelement_FV2304</t>
+  </si>
+  <si>
+    <t>Segment ID_FV2304</t>
+  </si>
+  <si>
+    <t>Code_FV2304</t>
+  </si>
+  <si>
+    <t>Qualifier_FV2304</t>
+  </si>
+  <si>
+    <t>Beschreibung_FV2304</t>
+  </si>
+  <si>
+    <t>Bedingungsausdruck_FV2304</t>
+  </si>
+  <si>
+    <t>Bedingung_FV2304</t>
   </si>
   <si>
     <t>Nachrichten-Kopfsegment</t>
@@ -675,6 +675,36 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:U74" totalsRowShown="0">
+  <autoFilter ref="A1:U74"/>
+  <tableColumns count="21">
+    <tableColumn id="1" name="Segmentname_FV2210"/>
+    <tableColumn id="2" name="Segmentgruppe_FV2210"/>
+    <tableColumn id="3" name="Segment_FV2210"/>
+    <tableColumn id="4" name="Datenelement_FV2210"/>
+    <tableColumn id="5" name="Segment ID_FV2210"/>
+    <tableColumn id="6" name="Code_FV2210"/>
+    <tableColumn id="7" name="Qualifier_FV2210"/>
+    <tableColumn id="8" name="Beschreibung_FV2210"/>
+    <tableColumn id="9" name="Bedingungsausdruck_FV2210"/>
+    <tableColumn id="10" name="Bedingung_FV2210"/>
+    <tableColumn id="11" name="diff"/>
+    <tableColumn id="12" name="Segmentname_FV2304"/>
+    <tableColumn id="13" name="Segmentgruppe_FV2304"/>
+    <tableColumn id="14" name="Segment_FV2304"/>
+    <tableColumn id="15" name="Datenelement_FV2304"/>
+    <tableColumn id="16" name="Segment ID_FV2304"/>
+    <tableColumn id="17" name="Code_FV2304"/>
+    <tableColumn id="18" name="Qualifier_FV2304"/>
+    <tableColumn id="19" name="Beschreibung_FV2304"/>
+    <tableColumn id="20" name="Bedingungsausdruck_FV2304"/>
+    <tableColumn id="21" name="Bedingung_FV2304"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -964,7 +994,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4393,5 +4426,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Regenerate compared AHB files
</commit_message>
<xml_diff>
--- a/data/output/FV2304_FV2210/COMDIS/29001.xlsx
+++ b/data/output/FV2304_FV2210/COMDIS/29001.xlsx
@@ -1323,7 +1323,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="2"/>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N9" s="2"/>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="N12" s="2"/>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N15" s="2"/>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N19" s="2"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N23" s="2" t="s">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="2" t="s">
+      <c r="M29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="N29" s="2" t="s">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N32" s="2" t="s">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N39" s="2" t="s">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="2" t="s">
+      <c r="M45" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N45" s="2" t="s">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="2" t="s">
+      <c r="M49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N49" s="2" t="s">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="2" t="s">
+      <c r="M52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N52" s="2" t="s">
@@ -3989,7 +3989,7 @@
         <v>188</v>
       </c>
       <c r="L57" s="4"/>
-      <c r="M57" s="2" t="s">
+      <c r="M57" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N57" s="2" t="s">
@@ -4621,7 +4621,7 @@
         <v>190</v>
       </c>
       <c r="L69" s="4"/>
-      <c r="M69" s="2" t="s">
+      <c r="M69" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N69" s="2" t="s">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="2" t="s">
+      <c r="M72" s="3" t="s">
         <v>36</v>
       </c>
       <c r="N72" s="2"/>

</xml_diff>

<commit_message>
chore: ensure consistent formatting of highlighted entries (#21)
* Make changing `Segmentname` bold regardless of cell formatting

* Overwrite grey cells with highlighted changes

* Apply background only if row is not already affected by any highlighting

* Regenerate compared AHB files

* Improve readme formatting
</commit_message>
<xml_diff>
--- a/data/output/FV2304_FV2210/COMDIS/29001.xlsx
+++ b/data/output/FV2304_FV2210/COMDIS/29001.xlsx
@@ -1323,7 +1323,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="2"/>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="2" t="s">
+      <c r="M9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N9" s="2"/>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="N12" s="2"/>
@@ -1929,7 +1929,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="N15" s="2"/>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="2" t="s">
+      <c r="M19" s="3" t="s">
         <v>26</v>
       </c>
       <c r="N19" s="2"/>
@@ -2305,7 +2305,7 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="2" t="s">
+      <c r="M23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="N23" s="2" t="s">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="K29" s="2"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="2" t="s">
+      <c r="M29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="N29" s="2" t="s">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="2" t="s">
+      <c r="M32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N32" s="2" t="s">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="2" t="s">
+      <c r="M39" s="3" t="s">
         <v>30</v>
       </c>
       <c r="N39" s="2" t="s">
@@ -3405,7 +3405,7 @@
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="2" t="s">
+      <c r="M45" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N45" s="2" t="s">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="2" t="s">
+      <c r="M49" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N49" s="2" t="s">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="4"/>
-      <c r="M52" s="2" t="s">
+      <c r="M52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="N52" s="2" t="s">
@@ -3989,7 +3989,7 @@
         <v>188</v>
       </c>
       <c r="L57" s="4"/>
-      <c r="M57" s="2" t="s">
+      <c r="M57" s="3" t="s">
         <v>34</v>
       </c>
       <c r="N57" s="2" t="s">
@@ -4621,7 +4621,7 @@
         <v>190</v>
       </c>
       <c r="L69" s="4"/>
-      <c r="M69" s="2" t="s">
+      <c r="M69" s="3" t="s">
         <v>35</v>
       </c>
       <c r="N69" s="2" t="s">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="K72" s="2"/>
       <c r="L72" s="4"/>
-      <c r="M72" s="2" t="s">
+      <c r="M72" s="3" t="s">
         <v>36</v>
       </c>
       <c r="N72" s="2"/>

</xml_diff>